<commit_message>
Signed-off-by: LECTURER Robert Sheehy <lt00036625@365s.ittralee.ie>
</commit_message>
<xml_diff>
--- a/Assignment Briefs/Assignment 1.xlsx
+++ b/Assignment Briefs/Assignment 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lt00036625\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lt00036625\Desktop\Computer Graphics\Assignment Briefs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1752A1F-D1E1-432D-9A09-3CF337E3768D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1097394-B404-4A81-ADF1-AE2EB1DA06CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
@@ -530,31 +530,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -562,6 +547,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -581,6 +581,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201706</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>776386</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1640182</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C443CF35-4AE0-4DC9-801B-A9718B044E23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2386853" y="6017559"/>
+          <a:ext cx="2715004" cy="1438476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1036813</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1725707</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76A3737C-B25E-4F39-81CF-1B38D7A82DB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1815353" y="313766"/>
+          <a:ext cx="3546931" cy="1725706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -906,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1133,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1158,10 +1251,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1172,8 +1265,8 @@
     </row>
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="33"/>
       <c r="G3" s="11"/>
       <c r="H3" s="34"/>
@@ -1193,10 +1286,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1205,8 +1298,8 @@
     </row>
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1226,10 +1319,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1239,8 +1332,8 @@
     </row>
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1260,28 +1353,28 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="48"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1301,10 +1394,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1316,8 +1409,8 @@
     </row>
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1341,10 +1434,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1356,8 +1449,8 @@
     </row>
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1378,18 +1471,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="41"/>
       <c r="F20" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="46"/>
-      <c r="H20" s="47" t="s">
+      <c r="G20" s="45"/>
+      <c r="H20" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="48"/>
+      <c r="I20" s="43"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1397,12 +1490,12 @@
     </row>
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="44"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1420,33 +1513,33 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="47" t="s">
+      <c r="L23" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="48"/>
+      <c r="M23" s="43"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="43"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="39"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1459,10 +1552,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="48"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1473,8 +1566,8 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1492,15 +1585,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="48"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="39"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1511,11 +1604,11 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="B30" s="43"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1533,44 +1626,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="39"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="38" t="s">
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="39"/>
+      <c r="M32" s="41"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="46"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="39"/>
       <c r="F33" s="44"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="41"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="46"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1582,33 +1675,46 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="48"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="43"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="39"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="41"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -1625,29 +1731,17 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>